<commit_message>
Started using unit mechanics for unit cohesion rather than relying on the selectable_models tag. Added __str__ functions for army, unit which are called on new game. Added Plague Marines to the spreadsheet, made them the default enemy. Selectable models are now generated through the map just like the targets and walls.
</commit_message>
<xml_diff>
--- a/pygame/40k_sim_workbook.xlsx
+++ b/pygame/40k_sim_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B327F5B1-B353-4E9D-A98D-6A7E2F936364}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A67486A-638E-4631-A641-CF737ECD6134}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="2" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Weapon</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Radius</t>
+  </si>
+  <si>
+    <t>Plague Marine</t>
+  </si>
+  <si>
+    <t>Plague Champion</t>
   </si>
 </sst>
 </file>
@@ -1505,11 +1511,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC9FF83-A4B4-495A-8CD6-852B5A72C621}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,6 +1807,76 @@
         <v>6</v>
       </c>
       <c r="L10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="L14">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented basic model selection in charge phase. Added special movement flags to sprites. Made FPS counter int rather than float. Added charge phase section to sprite.update() as well as charge distance trackers, but haven't implemented actual movement yet.
</commit_message>
<xml_diff>
--- a/pygame/40k_sim_workbook.xlsx
+++ b/pygame/40k_sim_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A67486A-638E-4631-A641-CF737ECD6134}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDE814A-011D-41D5-9621-E032F05E42FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="2" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Templar Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Templar Models" sheetId="2" r:id="rId3"/>
     <sheet name="Army Sheet" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDAFB37-BC4F-43E6-8574-A43CDCD4006E}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC9FF83-A4B4-495A-8CD6-852B5A72C621}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>

</xml_diff>

<commit_message>
Segregated melee weapons and ranged weapons in all cases in preparation of Fight Phase implementation.
</commit_message>
<xml_diff>
--- a/pygame/40k_sim_workbook.xlsx
+++ b/pygame/40k_sim_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDE814A-011D-41D5-9621-E032F05E42FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01311684-421D-44EA-ABCF-294CF2F6B71A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="1" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Templar Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Weapon</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Plague Champion</t>
+  </si>
+  <si>
+    <t>CCW</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -355,6 +358,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,9 +683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDAFB37-BC4F-43E6-8574-A43CDCD4006E}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,14 +1382,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9B6098-EF80-434F-8A4C-B8A7BE87648E}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="18"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
@@ -1386,92 +1399,104 @@
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="15">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="C1" s="15">
+        <v>3</v>
+      </c>
+      <c r="D1" s="15">
+        <v>4</v>
+      </c>
+      <c r="E1" s="15">
+        <v>5</v>
+      </c>
+      <c r="F1" s="15">
+        <v>6</v>
+      </c>
+      <c r="G1" s="15">
+        <v>7</v>
+      </c>
+      <c r="H1" s="15">
+        <v>8</v>
+      </c>
+      <c r="I1" s="15">
+        <v>9</v>
+      </c>
+      <c r="J1" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="8">
-        <v>-3</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+        <v>59</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
@@ -1480,6 +1505,43 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>